<commit_message>
Adding new sprint plan
</commit_message>
<xml_diff>
--- a/statistics/burndown-chart.xlsx
+++ b/statistics/burndown-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\Github\artifacts\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD3340C-3208-4F4F-99D3-276B8A29C9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F5FFB4-BA0F-4BF4-86E6-2CB7418B2FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6FFFC4D-3734-4703-94AD-2D56345C9C21}"/>
   </bookViews>
@@ -3301,7 +3301,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>